<commit_message>
reset date button init
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -406,12 +406,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t xml:space="preserve">127.58
+          <t xml:space="preserve">81.32
 </t>
         </is>
       </c>
@@ -424,12 +424,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">81.32
+          <t xml:space="preserve">127.58
 </t>
         </is>
       </c>

</xml_diff>